<commit_message>
SAG Sagemaker XGBoost Results WIP
</commit_message>
<xml_diff>
--- a/data/sag2/SAG Local LSTM Testing Results.xlsx
+++ b/data/sag2/SAG Local LSTM Testing Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/sag2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED83DC7-2853-0442-BFE3-948E0C74B636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032FFAE6-D1C4-DA40-A666-7FC40D7223C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="1120" windowWidth="38960" windowHeight="26140" xr2:uid="{98773DA3-37B5-D741-8ED4-95FED174B96A}"/>
   </bookViews>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1097,7 +1097,7 @@
     <col min="14" max="14" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="15" max="16" width="8.6640625" customWidth="1"/>
     <col min="17" max="20" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="8" style="1" customWidth="1"/>
     <col min="23" max="23" width="8.33203125" style="1" customWidth="1"/>
     <col min="24" max="24" width="34.1640625" style="2" customWidth="1"/>

</xml_diff>